<commit_message>
updated ehic dataset + changed the views for the issuance
</commit_message>
<xml_diff>
--- a/wallet-enterprise-configurations/ehic-issuer/dataset/ehic-dataset.xlsx
+++ b/wallet-enterprise-configurations/ehic-issuer/dataset/ehic-dataset.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koukoularism/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D478C72-37F8-B042-9F30-17D36C3EA741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC6796C3-3BE9-F140-A3C7-1B7D2E82B377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="1500" windowWidth="27640" windowHeight="16440" xr2:uid="{BE1A1EF8-ED33-F949-9E16-D8760E6AF670}"/>
   </bookViews>
   <sheets>
     <sheet name="EHIC" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
-  <si>
-    <t>pid_id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>2035-04-21</t>
   </si>
@@ -84,6 +81,18 @@
   </si>
   <si>
     <t>Jones</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>issuer_institution_code</t>
+  </si>
+  <si>
+    <t>issuer_country</t>
   </si>
 </sst>
 </file>
@@ -121,7 +130,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -212,14 +221,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -229,11 +269,74 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -428,17 +531,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B04C754A-41DE-1A4A-87B4-913642A7E9F9}" name="Table1" displayName="Table1" ref="A1:H3" totalsRowShown="0" tableBorderDxfId="7">
-  <autoFilter ref="A1:H3" xr:uid="{B04C754A-41DE-1A4A-87B4-913642A7E9F9}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{595573F7-8F16-4944-B69A-7F51A06ED9DA}" name="pid_id" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{9E62065E-FE56-8243-B404-6EDDDECBFFF9}" name="expiry_date" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{CBBF3AC5-58E9-7043-84DA-BE34AEFD4300}" name="family_name" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{07ACEB2A-30B6-164B-B639-D8B494EFCF49}" name="given_name" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{EC279AFD-A628-194B-88BC-809FF0B80C11}" name="birth_date" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{F2694451-3C25-BF4C-9B0D-870390F9C3B3}" name="ssn" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{7281D98B-3791-4340-B706-3E31F428795B}" name="User" dataDxfId="0"/>
-    <tableColumn id="11" xr3:uid="{BDBE97FF-02B2-9B43-AD12-3AE793694252}" name="Password"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B04C754A-41DE-1A4A-87B4-913642A7E9F9}" name="Table1" displayName="Table1" ref="A1:J3" totalsRowShown="0" tableBorderDxfId="9">
+  <autoFilter ref="A1:J3" xr:uid="{B04C754A-41DE-1A4A-87B4-913642A7E9F9}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{595573F7-8F16-4944-B69A-7F51A06ED9DA}" name="id" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{9E62065E-FE56-8243-B404-6EDDDECBFFF9}" name="expiry_date" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{CBBF3AC5-58E9-7043-84DA-BE34AEFD4300}" name="family_name" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{07ACEB2A-30B6-164B-B639-D8B494EFCF49}" name="given_name" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{EC279AFD-A628-194B-88BC-809FF0B80C11}" name="birth_date" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{F2694451-3C25-BF4C-9B0D-870390F9C3B3}" name="ssn" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{7281D98B-3791-4340-B706-3E31F428795B}" name="issuer_country" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{BDBE97FF-02B2-9B43-AD12-3AE793694252}" name="issuer_institution_code" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{57057B67-4667-7848-A879-0C6EB098AEA1}" name="User" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{5C4B7C02-32F5-864F-BA7A-26EA616ED0CC}" name="Password"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -761,10 +866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C96A804-F114-CB45-8EC0-CCF09274E1D5}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -778,82 +883,100 @@
     <col min="11" max="11" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="7">
+        <v>33161</v>
+      </c>
+      <c r="F2" s="8">
+        <v>12313213213</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="14">
+        <v>2</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="7">
+        <v>33161</v>
+      </c>
+      <c r="F3" s="9">
+        <v>52313313216</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="14">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="9">
-        <v>33161</v>
-      </c>
-      <c r="F2" s="10">
-        <v>12313213213</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="I3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="11" t="s">
         <v>4</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="9">
-        <v>33161</v>
-      </c>
-      <c r="F3" s="11">
-        <v>52313313216</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>